<commit_message>
controls should be sorted
</commit_message>
<xml_diff>
--- a/NNC-AWS-Confg.xlsx
+++ b/NNC-AWS-Confg.xlsx
@@ -535,7 +535,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -546,12 +546,12 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>AC-03_S3_Account_Level_Public_Access_Blocks</t>
+          <t>AC-02_Access_Keys_Rotated</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Checks whether the required public access block settings are configured from account level. The rule is NON_COMPLIANT when the public access block settings are not configured from account level.</t>
+          <t>Checks whether the active access keys are rotated within the number of days specified in maxAccessKeyAge. The rule is non-compliant if the access keys have not been rotated for more than maxAccessKeyAge number of days.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -563,28 +563,28 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IA</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>IA-2</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Identification and Authentication</t>
+          <t>Access Control</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>IA-02_IAM_Password_Policy</t>
+          <t>AC-02_Cloud_Trail_Cloud_Watch_Logs_Enabled</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Checks whether the account password policy for IAM users meets the specified requirements indicated in the parameters. This rule is NON_COMPLIANT if the account password policy does not meet the specified requirements.</t>
+          <t>Checks whether AWS CloudTrail trails are configured to send logs to Amazon CloudWatch logs. The trail is non-compliant if the CloudWatchLogsLogGroupArn property of the trail is empty.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -601,7 +601,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AC-17(3)</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -612,12 +612,12 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>AC-17-03_Internet_Gateway_Authorized_VPC_Only</t>
+          <t>AC-02_Cloud_Trail_Enabled</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Checks that Internet gateways (IGWs) are only attached to an authorized Amazon Virtual Private Cloud (VPCs). The rule is NON_COMPLIANT if IGWs are not attached to an authorized VPC.</t>
+          <t>Checks whether AWS CloudTrail is enabled in your AWS account.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -634,7 +634,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -645,12 +645,12 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>AC-03_IAM_User_No_Policies_Check</t>
+          <t>AC-02_Cloudtrail_S3_Dataevents_Enabled</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Checks that none of your IAM users have policies attached. IAM users must inherit permissions from IAM groups or roles.</t>
+          <t>Checks whether at least one AWS CloudTrail trail is logging Amazon S3 data events for all S3 buckets. The rule is NON_COMPLIANT if trails log data events for S3 buckets is not configured.</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -667,7 +667,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AC-17(2)</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -678,12 +678,12 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>AC-17-02_ELB_ACM_Certificate_Required</t>
+          <t>AC-02_Cloudwatch_Alarm_Action_Check</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>This rule checks whether the Elastic Load Balancer(s) uses SSL certificates provided by AWS Certificate Manager. You must use an SSL or HTTPS listener with your Elastic Load Balancer to use this rule.</t>
+          <t>Checks whether CloudWatch alarms have at least one alarm action, one INSUFFICIENT_DATA action, or one OK action enabled. Optionally, checks whether any of the actions matches one of the specified ARNs.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -700,7 +700,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AC-17(1)</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -711,12 +711,12 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>AC-17-01_Guardduty_Enabled_Centralized</t>
+          <t>AC-02_EMR_Kerberos_Enabled</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Checks whether GuardDuty is enabled. You can optionally verify that the results are centralized in a specific AWS Account.</t>
+          <t>The rule is NON_COMPLIANT if a security configuration is not attached to the cluster or the security configuration does not satisfy the specified rule parameters.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -744,12 +744,12 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>AC-02_IAM_Password_Policy</t>
+          <t>AC-02_Guardduty_Enabled_Centralized</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Checks whether the account password policy for IAM users meets the specified requirements indicated in the parameters. This rule is NON_COMPLIANT if the account password policy does not meet the specified requirements.</t>
+          <t>Checks whether GuardDuty is enabled. You can optionally verify that the results are centralized in a specific AWS Account.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -777,12 +777,12 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>AC-02_S3_Bucket_Logging_Enabled</t>
+          <t>AC-02_IAM_Group_Has_Users_Check</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Checks whether logging is enabled for your S3 buckets.</t>
+          <t>Checks whether IAM groups have at least one IAM user.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -810,12 +810,12 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>AC-02_IAM_User_Unused_Credentials_Check</t>
+          <t>AC-02_IAM_Password_Policy</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Checks whether your AWS Identity and Access Management (IAM) users have passwords or active access keys that have not been used within the specified number of days you provided.</t>
+          <t>Checks whether the account password policy for IAM users meets the specified requirements indicated in the parameters. This rule is NON_COMPLIANT if the account password policy does not meet the specified requirements.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -843,12 +843,12 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>AC-02_Cloud_Trail_Enabled</t>
+          <t>AC-02_IAM_Policy_No_Statements_With_Admin_Access</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Checks whether AWS CloudTrail is enabled in your AWS account.</t>
+          <t>Checks whether the default version of AWS Identity and Access Management (IAM) policies do not have administrator access. If any statement has "Effect": "Allow" with "Action": "*" over "Resource": "*", the rule is non-compliant.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -876,12 +876,12 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>AC-02_Redshift_Cluster_Configuration_Check</t>
+          <t>AC-02_IAM_Root_Access_Key_Check</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Checks whether Amazon Redshift clusters have the specified settings.</t>
+          <t>Checks whether the root user access key is available. The rule is compliant if the user access key does not exist.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -893,28 +893,28 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CM-8(3)</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Configuration Management</t>
+          <t>Access Control</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>CM-08-03_EC2_Managedinstance_Association_Compliance_Status_Check</t>
+          <t>AC-02_IAM_User_Group_Membership_Check</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Checks whether the compliance status of the AWS Systems Manager association compliance is COMPLIANT or NON_COMPLIANT after the association execution on the instance. The rule is compliant if the field status is COMPLIANT.</t>
+          <t>Checks whether IAM users are members of at least one IAM group.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -926,28 +926,28 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CM-8(3)</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Configuration Management</t>
+          <t>Access Control</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>CM-08-03_EC2_Managedinstance_Patch_Compliance_Status_Check</t>
+          <t>AC-02_IAM_User_No_Policies_Check</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Checks whether the compliance status of the AWS Systems Manager patch compliance is COMPLIANT or NON_COMPLIANT after the patch installation on the instance. The rule is compliant if the field status is COMPLIANT.</t>
+          <t>Checks that none of your IAM users have policies attached. IAM users must inherit permissions from IAM groups or roles.</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -975,12 +975,12 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>AC-02_Secretsmanager_Scheduled_Rotation_Success_Check</t>
+          <t>AC-02_IAM_User_Unused_Credentials_Check</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Checks whether AWS Secrets Manager secret rotation has rotated successfully as per the rotation schedule. The rule returns NON_COMPLIANT if RotationOccurringAsScheduled is false.</t>
+          <t>Checks whether your AWS Identity and Access Management (IAM) users have passwords or active access keys that have not been used within the specified number of days you provided.</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -997,7 +997,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AC-17(2)</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1008,12 +1008,12 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>AC-17-02_ALB_HTTP_Drop_Invalid_Header_Enabled</t>
+          <t>AC-02_Multi_Region_Cloudtrail_Enabled</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Checks if rule evaluates AWS Application Load Balancers (ALB) to ensure they are configured to drop http headers. The rule is NON_COMPLIANT if the value of routing.http.drop_invalid_header_fields.enabled is set to false.</t>
+          <t>Checks that there is at least one multi-region AWS CloudTrail. The rule is non-compliant if the trails do not match input parameters</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1041,12 +1041,12 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>AC-03_Sagemaker_Notebook_No_Direct_Internet_Access</t>
+          <t>AC-02_RDS_Logging_Enabled</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Checks whether direct internet access is disabled for an Amazon SageMaker notebook instance. The rule is NON_COMPLIANT if Amazon SageMaker notebook instances are internet-enabled.</t>
+          <t>Checks that respective logs of Amazon Relational Database Service (Amazon RDS) are enabled. The rule is NON_COMPLIANT if any log types are not enabled.</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AC-6(10)</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1074,12 +1074,12 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>AC-06-10_IAM_Root_Access_Key_Check</t>
+          <t>AC-02_Redshift_Cluster_Configuration_Check</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Checks whether the root user access key is available. The rule is compliant if the user access key does not exist.</t>
+          <t>Checks whether Amazon Redshift clusters have the specified settings.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1107,12 +1107,12 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>AC-03_IAM_User_Group_Membership_Check</t>
+          <t>AC-02_S3_Bucket_Logging_Enabled</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Checks whether IAM users are members of at least one IAM group.</t>
+          <t>Checks whether logging is enabled for your S3 buckets.</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AC-17(2)</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1140,12 +1140,12 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>AC-17-02_Redshift_Require_TLS_SSL</t>
+          <t>AC-02_Secretsmanager_Scheduled_Rotation_Success_Check</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Checks whether Amazon Redshift clusters require TLS/SSL encryption to connect to SQL clients. The rule is NON_COMPLIANT if any Amazon Redshift cluster has parameter require_SSL not set to true.</t>
+          <t>Checks whether AWS Secrets Manager secret rotation has rotated successfully as per the rotation schedule. The rule returns NON_COMPLIANT if RotationOccurringAsScheduled is false.</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AC-2</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1173,12 +1173,12 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>AC-03_S3_Bucket_Policy_Grantee_Check</t>
+          <t>AC-02_Securityhub_Enabled</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Checks that the access granted by the Amazon S3 bucket is restricted to any of the AWS principals, federated users, service principals, IP addresses, or VPCs that you provide. The rule is COMPLIANT if a bucket policy is not present.</t>
+          <t>Checks that AWS Security Hub is enabled for an AWS Account. The rule is NON_COMPLIANT if AWS Security Hub is not enabled.</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1206,12 +1206,12 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>AC-02_IAM_Group_Has_Users_Check</t>
+          <t>AC-03_DMS_Replication_Not_Public</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Checks whether IAM groups have at least one IAM user.</t>
+          <t>Checks whether AWS Database Migration Service replication instances are public. The rule is NON_COMPLIANT if PubliclyAccessible field is True.</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1239,12 +1239,12 @@
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>AC-03_IAM_User_Unused_Credentials_Check</t>
+          <t>AC-03_EBS_Snapshot_Public_Restorable_Check</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Checks whether your AWS Identity and Access Management (IAM) users have passwords or active access keys that have not been used within the specified number of days you provided.</t>
+          <t>Checks whether Amazon Elastic Block Store (Amazon EBS) snapshots are not publicly restorable. The rule is NON_COMPLIANT if one or more snapshots with RestorableByUserIds field are set to all, that is, Amazon EBS snapshots are public.</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1272,12 +1272,12 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>AC-02_IAM_User_No_Policies_Check</t>
+          <t>AC-03_EMR_Kerberos_Enabled</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Checks that none of your IAM users have policies attached. IAM users must inherit permissions from IAM groups or roles.</t>
+          <t>The rule is NON_COMPLIANT if a security configuration is not attached to the cluster or the security configuration does not satisfy the specified rule parameters.</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1289,28 +1289,28 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>AU-9</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Audit and Accountability</t>
+          <t>Access Control</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>AU-09_Cloudwatch_Log_Group_Encrypted</t>
+          <t>AC-03_IAM_Group_Has_Users_Check</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Checks whether a log group in Amazon CloudWatch Logs is encrypted. The rule is NON_COMPLIANT if CloudWatch Logs has log group without encryption enabled.</t>
+          <t>Checks whether IAM groups have at least one IAM user.</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1338,12 +1338,12 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>AC-02_IAM_Root_Access_Key_Check</t>
+          <t>AC-03_IAM_Policy_No_Statements_With_Admin_Access</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Checks whether the root user access key is available. The rule is compliant if the user access key does not exist.</t>
+          <t>Checks whether the default version of AWS Identity and Access Management (IAM) policies do not have administrator access. If any statement has "Effect": "Allow" with "Action": "*" over "Resource": "*", the rule is non-compliant.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1371,12 +1371,12 @@
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>AC-03_Lambda_Function_Public_Access_Prohibited</t>
+          <t>AC-03_IAM_Root_Access_Key_Check</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Checks whether the Lambda function policy prohibits public access.</t>
+          <t>Checks whether the root user access key is available. The rule is compliant if the user access key does not exist.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1404,12 +1404,12 @@
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>AC-02_Access_Keys_Rotated</t>
+          <t>AC-03_IAM_User_Group_Membership_Check</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Checks whether the active access keys are rotated within the number of days specified in maxAccessKeyAge. The rule is non-compliant if the access keys have not been rotated for more than maxAccessKeyAge number of days.</t>
+          <t>Checks whether IAM users are members of at least one IAM group.</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1437,12 +1437,12 @@
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>AC-02_IAM_User_Group_Membership_Check</t>
+          <t>AC-03_IAM_User_No_Policies_Check</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Checks whether IAM users are members of at least one IAM group.</t>
+          <t>Checks that none of your IAM users have policies attached. IAM users must inherit permissions from IAM groups or roles.</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1470,12 +1470,12 @@
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>AC-03_EBS_Snapshot_Public_Restorable_Check</t>
+          <t>AC-03_IAM_User_Unused_Credentials_Check</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Checks whether Amazon Elastic Block Store (Amazon EBS) snapshots are not publicly restorable. The rule is NON_COMPLIANT if one or more snapshots with RestorableByUserIds field are set to all, that is, Amazon EBS snapshots are public.</t>
+          <t>Checks whether your AWS Identity and Access Management (IAM) users have passwords or active access keys that have not been used within the specified number of days you provided.</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1485,12 +1485,32 @@
       <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>AC</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>AC-3</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Access Control</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>AC-03_Lambda_Function_Public_Access_Prohibited</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Checks whether the Lambda function policy prohibits public access.</t>
+        </is>
+      </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
@@ -1505,7 +1525,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>AC-17(2)</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1516,12 +1536,12 @@
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>AC-17-02_ALB_HTTP_To_HTTPS_Redirection_Check</t>
+          <t>AC-03_RDS_Snapshots_Public_Prohibited</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Checks whether HTTP to HTTPS redirection is configured on all HTTP listeners of Application Load Balancers. The rule is NON_COMPLIANT if one or more HTTP listeners of Application Load Balancer do not have HTTP to HTTPS redirection configured.</t>
+          <t>AC-03_RDS_Snapshots_Public_Prohibited</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -1533,28 +1553,28 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>CM-7</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Configuration Management</t>
+          <t>Access Control</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>CM-07_EC2_Managedinstance_Association_Compliance_Status_Check</t>
+          <t>AC-03_Redshift_Cluster_Public_Access_Check</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Checks whether the compliance status of the AWS Systems Manager association compliance is COMPLIANT or NON_COMPLIANT after the association execution on the instance. The rule is compliant if the field status is COMPLIANT.</t>
+          <t>Checks whether Amazon Redshift clusters are not publicly accessible. The rule is NON_COMPLIANT if the publicly accessible field is true in the cluster configuration item.</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -1582,12 +1602,12 @@
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>AC-03_IAM_Root_Access_Key_Check</t>
+          <t>AC-03_S3_Account_Level_Public_Access_Blocks</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Checks whether the root user access key is available. The rule is compliant if the user access key does not exist.</t>
+          <t>Checks whether the required public access block settings are configured from account level. The rule is NON_COMPLIANT when the public access block settings are not configured from account level.</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -1615,12 +1635,12 @@
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>AC-03_DMS_Replication_Not_Public</t>
+          <t>AC-03_S3_Bucket_Policy_Grantee_Check</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Checks whether AWS Database Migration Service replication instances are public. The rule is NON_COMPLIANT if PubliclyAccessible field is True.</t>
+          <t>Checks that the access granted by the Amazon S3 bucket is restricted to any of the AWS principals, federated users, service principals, IP addresses, or VPCs that you provide. The rule is COMPLIANT if a bucket policy is not present.</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -1637,7 +1657,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1648,12 +1668,12 @@
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>AC-02_EMR_Kerberos_Enabled</t>
+          <t>AC-03_S3_Bucket_Public_Write_Prohibited</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>The rule is NON_COMPLIANT if a security configuration is not attached to the cluster or the security configuration does not satisfy the specified rule parameters.</t>
+          <t>Checks that your Amazon S3 buckets do not allow public write access. The rule checks the Block Public Access settings, the bucket policy, and the bucket access control list (ACL).</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -1681,12 +1701,12 @@
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>AC-03_IAM_Policy_No_Statements_With_Admin_Access</t>
+          <t>AC-03_Sagemaker_Notebook_No_Direct_Internet_Access</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Checks whether the default version of AWS Identity and Access Management (IAM) policies do not have administrator access. If any statement has "Effect": "Allow" with "Action": "*" over "Resource": "*", the rule is non-compliant.</t>
+          <t>Checks whether direct internet access is disabled for an Amazon SageMaker notebook instance. The rule is NON_COMPLIANT if Amazon SageMaker notebook instances are internet-enabled.</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -1703,7 +1723,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AC-6(10)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1714,12 +1734,12 @@
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>AC-02_RDS_Logging_Enabled</t>
+          <t>AC-06-10_IAM_Root_Access_Key_Check</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Checks that respective logs of Amazon Relational Database Service (Amazon RDS) are enabled. The rule is NON_COMPLIANT if any log types are not enabled.</t>
+          <t>Checks whether the root user access key is available. The rule is compliant if the user access key does not exist.</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -1736,7 +1756,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AC-17(1)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1747,12 +1767,12 @@
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>AC-03_IAM_Group_Has_Users_Check</t>
+          <t>AC-17-01_Guardduty_Enabled_Centralized</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Checks whether IAM groups have at least one IAM user.</t>
+          <t>Checks whether GuardDuty is enabled. You can optionally verify that the results are centralized in a specific AWS Account.</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -1764,28 +1784,28 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>CM-8(3)</t>
+          <t>AC-17(1)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Configuration Management</t>
+          <t>Access Control</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>CM-08-03_EC2_Instance_Managed_By_Systems_Manager</t>
+          <t>AC-17-01_Securityhub_Enabled</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Checks whether the Amazon EC2 instances in your account are managed by AWS Systems Manager.</t>
+          <t>Checks that AWS Security Hub is enabled for an AWS Account. The rule is NON_COMPLIANT if AWS Security Hub is not enabled.</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -1797,28 +1817,28 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>AU-9</t>
+          <t>AC-17(2)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Audit and Accountability</t>
+          <t>Access Control</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>AU-09_Cloud_Trail_Encryption_Enabled</t>
+          <t>AC-17-02_ACM_Certificate_Expiration_Check</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Checks whether AWS CloudTrail is configured to use the server side encryption (SSE) AWS Key Management Service (AWS KMS) customer master key (CMK) encryption. The rule is compliant if the KmsKeyId is defined.</t>
+          <t>Checks whether ACM Certificates in your account are marked for expiration within the specified number of days. Certificates provided by ACM are automatically renewed. ACM does not automatically renew certificates that you import.</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -1830,28 +1850,28 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>AC</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>CM-7</t>
+          <t>AC-17(2)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Configuration Management</t>
+          <t>Access Control</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>CM-07_EC2_Instance_Managed_By_Systems_Manager</t>
+          <t>AC-17-02_ALB_HTTP_Drop_Invalid_Header_Enabled</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Checks whether the Amazon EC2 instances in your account are managed by AWS Systems Manager.</t>
+          <t>Checks if rule evaluates AWS Application Load Balancers (ALB) to ensure they are configured to drop http headers. The rule is NON_COMPLIANT if the value of routing.http.drop_invalid_header_fields.enabled is set to false.</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -1868,7 +1888,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AC-17(2)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1879,12 +1899,12 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>AC-02_Guardduty_Enabled_Centralized</t>
+          <t>AC-17-02_ALB_HTTP_To_HTTPS_Redirection_Check</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Checks whether GuardDuty is enabled. You can optionally verify that the results are centralized in a specific AWS Account.</t>
+          <t>Checks whether HTTP to HTTPS redirection is configured on all HTTP listeners of Application Load Balancers. The rule is NON_COMPLIANT if one or more HTTP listeners of Application Load Balancer do not have HTTP to HTTPS redirection configured.</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -1912,12 +1932,12 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>AC-17-02_ELB_TLS_HTTPS_Listeners_Only</t>
+          <t>AC-17-02_ELB_ACM_Certificate_Required</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Checks whether your Classic Load Balancer's listeners are configured with SSL or HTTPS</t>
+          <t>This rule checks whether the Elastic Load Balancer(s) uses SSL certificates provided by AWS Certificate Manager. You must use an SSL or HTTPS listener with your Elastic Load Balancer to use this rule.</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -1934,7 +1954,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AC-17(2)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1945,12 +1965,12 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>AC-03_RDS_Snapshots_Public_Prohibited</t>
+          <t>AC-17-02_ELB_TLS_HTTPS_Listeners_Only</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>AC-03_RDS_Snapshots_Public_Prohibited</t>
+          <t>Checks whether your Classic Load Balancer's listeners are configured with SSL or HTTPS</t>
         </is>
       </c>
       <c r="G45" t="inlineStr"/>
@@ -1967,7 +1987,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AC-17(2)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1978,12 +1998,12 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>AC-03_S3_Bucket_Public_Write_Prohibited</t>
+          <t>AC-17-02_Redshift_Require_TLS_SSL</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Checks that your Amazon S3 buckets do not allow public write access. The rule checks the Block Public Access settings, the bucket policy, and the bucket access control list (ACL).</t>
+          <t>Checks whether Amazon Redshift clusters require TLS/SSL encryption to connect to SQL clients. The rule is NON_COMPLIANT if any Amazon Redshift cluster has parameter require_SSL not set to true.</t>
         </is>
       </c>
       <c r="G46" t="inlineStr"/>
@@ -2000,7 +2020,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AC-17(2)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2011,12 +2031,12 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>AC-02_Multi_Region_Cloudtrail_Enabled</t>
+          <t>AC-17-02_S3_Bucket_SSL_Requests_Only</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Checks that there is at least one multi-region AWS CloudTrail. The rule is non-compliant if the trails do not match input parameters</t>
+          <t>Checks whether S3 buckets have policies that require requests to use Secure Socket Layer (SSL).</t>
         </is>
       </c>
       <c r="G47" t="inlineStr"/>
@@ -2033,7 +2053,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>AC-17(1)</t>
+          <t>AC-17(3)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2044,12 +2064,12 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
-          <t>AC-17-01_Securityhub_Enabled</t>
+          <t>AC-17-03_Internet_Gateway_Authorized_VPC_Only</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Checks that AWS Security Hub is enabled for an AWS Account. The rule is NON_COMPLIANT if AWS Security Hub is not enabled.</t>
+          <t>Checks that Internet gateways (IGWs) are only attached to an authorized Amazon Virtual Private Cloud (VPCs). The rule is NON_COMPLIANT if IGWs are not attached to an authorized VPC.</t>
         </is>
       </c>
       <c r="G48" t="inlineStr"/>
@@ -2061,28 +2081,28 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AU-9</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Audit and Accountability</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>AC-03_EMR_Kerberos_Enabled</t>
+          <t>AU-09_Cloud_Trail_Encryption_Enabled</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>The rule is NON_COMPLIANT if a security configuration is not attached to the cluster or the security configuration does not satisfy the specified rule parameters.</t>
+          <t>Checks whether AWS CloudTrail is configured to use the server side encryption (SSE) AWS Key Management Service (AWS KMS) customer master key (CMK) encryption. The rule is compliant if the KmsKeyId is defined.</t>
         </is>
       </c>
       <c r="G49" t="inlineStr"/>
@@ -2094,28 +2114,28 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>AU</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>AU-9</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Audit and Accountability</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>AC-02_IAM_Policy_No_Statements_With_Admin_Access</t>
+          <t>AU-09_Cloudwatch_Log_Group_Encrypted</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Checks whether the default version of AWS Identity and Access Management (IAM) policies do not have administrator access. If any statement has "Effect": "Allow" with "Action": "*" over "Resource": "*", the rule is non-compliant.</t>
+          <t>Checks whether a log group in Amazon CloudWatch Logs is encrypted. The rule is NON_COMPLIANT if CloudWatch Logs has log group without encryption enabled.</t>
         </is>
       </c>
       <c r="G50" t="inlineStr"/>
@@ -2127,28 +2147,28 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>CM-7</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Configuration Management</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>AC-02_Cloud_Trail_Cloud_Watch_Logs_Enabled</t>
+          <t>CM-07_EC2_Instance_Managed_By_Systems_Manager</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Checks whether AWS CloudTrail trails are configured to send logs to Amazon CloudWatch logs. The trail is non-compliant if the CloudWatchLogsLogGroupArn property of the trail is empty.</t>
+          <t>Checks whether the Amazon EC2 instances in your account are managed by AWS Systems Manager.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr"/>
@@ -2160,28 +2180,28 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>AC-17(2)</t>
+          <t>CM-7</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Configuration Management</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>AC-17-02_ACM_Certificate_Expiration_Check</t>
+          <t>CM-07_EC2_Managedinstance_Association_Compliance_Status_Check</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Checks whether ACM Certificates in your account are marked for expiration within the specified number of days. Certificates provided by ACM are automatically renewed. ACM does not automatically renew certificates that you import.</t>
+          <t>Checks whether the compliance status of the AWS Systems Manager association compliance is COMPLIANT or NON_COMPLIANT after the association execution on the instance. The rule is compliant if the field status is COMPLIANT.</t>
         </is>
       </c>
       <c r="G52" t="inlineStr"/>
@@ -2193,28 +2213,28 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>CM-8(3)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Configuration Management</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>AC-03_Redshift_Cluster_Public_Access_Check</t>
+          <t>CM-08-03_EC2_Instance_Managed_By_Systems_Manager</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Checks whether Amazon Redshift clusters are not publicly accessible. The rule is NON_COMPLIANT if the publicly accessible field is true in the cluster configuration item.</t>
+          <t>Checks whether the Amazon EC2 instances in your account are managed by AWS Systems Manager.</t>
         </is>
       </c>
       <c r="G53" t="inlineStr"/>
@@ -2226,28 +2246,28 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>CM-8(3)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Configuration Management</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>AC-02_Cloudtrail_S3_Dataevents_Enabled</t>
+          <t>CM-08-03_EC2_Managedinstance_Association_Compliance_Status_Check</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Checks whether at least one AWS CloudTrail trail is logging Amazon S3 data events for all S3 buckets. The rule is NON_COMPLIANT if trails log data events for S3 buckets is not configured.</t>
+          <t>Checks whether the compliance status of the AWS Systems Manager association compliance is COMPLIANT or NON_COMPLIANT after the association execution on the instance. The rule is compliant if the field status is COMPLIANT.</t>
         </is>
       </c>
       <c r="G54" t="inlineStr"/>
@@ -2259,28 +2279,28 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>CM-8(3)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Configuration Management</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>AC-02_Cloudwatch_Alarm_Action_Check</t>
+          <t>CM-08-03_EC2_Managedinstance_Patch_Compliance_Status_Check</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Checks whether CloudWatch alarms have at least one alarm action, one INSUFFICIENT_DATA action, or one OK action enabled. Optionally, checks whether any of the actions matches one of the specified ARNs.</t>
+          <t>Checks whether the compliance status of the AWS Systems Manager patch compliance is COMPLIANT or NON_COMPLIANT after the patch installation on the instance. The rule is compliant if the field status is COMPLIANT.</t>
         </is>
       </c>
       <c r="G55" t="inlineStr"/>
@@ -2292,28 +2312,28 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>AC</t>
+          <t>IA</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>AC-2</t>
+          <t>IA-2</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Access Control</t>
+          <t>Identification and Authentication</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>AC-02_Securityhub_Enabled</t>
+          <t>IA-02_IAM_Password_Policy</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Checks that AWS Security Hub is enabled for an AWS Account. The rule is NON_COMPLIANT if AWS Security Hub is not enabled.</t>
+          <t>Checks whether the account password policy for IAM users meets the specified requirements indicated in the parameters. This rule is NON_COMPLIANT if the account password policy does not meet the specified requirements.</t>
         </is>
       </c>
       <c r="G56" t="inlineStr"/>
@@ -2323,32 +2343,12 @@
       <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>AC</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>AC-17(2)</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Access Control</t>
-        </is>
-      </c>
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>AC-17-02_S3_Bucket_SSL_Requests_Only</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Checks whether S3 buckets have policies that require requests to use Secure Socket Layer (SSL).</t>
-        </is>
-      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>

</xml_diff>

<commit_message>
Tagging and related generation
</commit_message>
<xml_diff>
--- a/NNC-AWS-Confg.xlsx
+++ b/NNC-AWS-Confg.xlsx
@@ -453,7 +453,7 @@
   <cols>
     <col width="17.5" customWidth="1" style="3" min="1" max="1"/>
     <col width="14.33203125" customWidth="1" style="3" min="2" max="2"/>
-    <col width="20.83203125" customWidth="1" style="4" min="3" max="3"/>
+    <col width="42.6640625" customWidth="1" style="4" min="3" max="3"/>
     <col width="66.1640625" customWidth="1" style="4" min="4" max="4"/>
     <col width="72.6640625" customWidth="1" style="4" min="5" max="5"/>
     <col width="61.5" customWidth="1" style="4" min="6" max="6"/>
@@ -569,11 +569,36 @@
           <t>Checks whether the active access keys are rotated within the number of days specified in maxAccessKeyAge. The rule is non-compliant if the access keys have not been rotated for more than maxAccessKeyAge number of days.</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -611,11 +636,36 @@
           <t>Checks whether AWS CloudTrail trails are configured to send logs to Amazon CloudWatch logs. The trail is non-compliant if the CloudWatchLogsLogGroupArn property of the trail is empty.</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -653,11 +703,36 @@
           <t>Checks whether AWS CloudTrail is enabled in your AWS account.</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -695,11 +770,36 @@
           <t>Checks whether at least one AWS CloudTrail trail is logging Amazon S3 data events for all S3 buckets. The rule is NON_COMPLIANT if trails log data events for S3 buckets is not configured.</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -737,11 +837,36 @@
           <t>Checks whether CloudWatch alarms have at least one alarm action, one INSUFFICIENT_DATA action, or one OK action enabled. Optionally, checks whether any of the actions matches one of the specified ARNs.</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -779,11 +904,36 @@
           <t>The rule is NON_COMPLIANT if a security configuration is not attached to the cluster or the security configuration does not satisfy the specified rule parameters.</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -821,11 +971,36 @@
           <t>Checks whether GuardDuty is enabled. You can optionally verify that the results are centralized in a specific AWS Account.</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -863,11 +1038,36 @@
           <t>Checks whether IAM groups have at least one IAM user.</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -905,11 +1105,36 @@
           <t>Checks whether the account password policy for IAM users meets the specified requirements indicated in the parameters. This rule is NON_COMPLIANT if the account password policy does not meet the specified requirements.</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -947,11 +1172,36 @@
           <t>Checks whether the default version of AWS Identity and Access Management (IAM) policies do not have administrator access. If any statement has "Effect": "Allow" with "Action": "*" over "Resource": "*", the rule is non-compliant.</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -989,11 +1239,36 @@
           <t>Checks whether the root user access key is available. The rule is compliant if the user access key does not exist.</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1031,11 +1306,36 @@
           <t>Checks whether IAM users are members of at least one IAM group.</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1073,11 +1373,36 @@
           <t>Checks that none of your IAM users have policies attached. IAM users must inherit permissions from IAM groups or roles.</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>AWS Managed</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>IAM</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Not Inherited</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>USNORTHCOM</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1115,11 +1440,36 @@
           <t>Checks whether your AWS Identity and Access Management (IAM) users have passwords or active access keys that have not been used within the specified number of days you provided.</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1157,11 +1507,36 @@
           <t>Checks that there is at least one multi-region AWS CloudTrail. The rule is non-compliant if the trails do not match input parameters</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1199,11 +1574,36 @@
           <t>Checks that respective logs of Amazon Relational Database Service (Amazon RDS) are enabled. The rule is NON_COMPLIANT if any log types are not enabled.</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1241,11 +1641,36 @@
           <t>Checks whether Amazon Redshift clusters have the specified settings.</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
-      <c r="L18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1283,11 +1708,36 @@
           <t>Checks whether logging is enabled for your S3 buckets.</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1325,11 +1775,36 @@
           <t>Checks whether AWS Secrets Manager secret rotation has rotated successfully as per the rotation schedule. The rule returns NON_COMPLIANT if RotationOccurringAsScheduled is false.</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1367,11 +1842,36 @@
           <t>Checks that AWS Security Hub is enabled for an AWS Account. The rule is NON_COMPLIANT if AWS Security Hub is not enabled.</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1409,11 +1909,36 @@
           <t>Checks whether AWS Database Migration Service replication instances are public. The rule is NON_COMPLIANT if PubliclyAccessible field is True.</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1451,11 +1976,36 @@
           <t>Checks whether Amazon Elastic Block Store (Amazon EBS) snapshots are not publicly restorable. The rule is NON_COMPLIANT if one or more snapshots with RestorableByUserIds field are set to all, that is, Amazon EBS snapshots are public.</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1493,11 +2043,36 @@
           <t>The rule is NON_COMPLIANT if a security configuration is not attached to the cluster or the security configuration does not satisfy the specified rule parameters.</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1535,11 +2110,36 @@
           <t>Checks whether IAM groups have at least one IAM user.</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1577,11 +2177,36 @@
           <t>Checks whether the default version of AWS Identity and Access Management (IAM) policies do not have administrator access. If any statement has "Effect": "Allow" with "Action": "*" over "Resource": "*", the rule is non-compliant.</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1619,11 +2244,36 @@
           <t>Checks whether the root user access key is available. The rule is compliant if the user access key does not exist.</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1661,11 +2311,36 @@
           <t>Checks whether IAM users are members of at least one IAM group.</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1703,11 +2378,36 @@
           <t>Checks that none of your IAM users have policies attached. IAM users must inherit permissions from IAM groups or roles.</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1745,11 +2445,36 @@
           <t>Checks whether your AWS Identity and Access Management (IAM) users have passwords or active access keys that have not been used within the specified number of days you provided.</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1787,11 +2512,36 @@
           <t>Checks whether the Lambda function policy prohibits public access.</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr"/>
-      <c r="L31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1829,11 +2579,36 @@
           <t>AC-03_RDS_Snapshots_Public_Prohibited</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1871,11 +2646,36 @@
           <t>Checks whether Amazon Redshift clusters are not publicly accessible. The rule is NON_COMPLIANT if the publicly accessible field is true in the cluster configuration item.</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1913,11 +2713,36 @@
           <t>Checks whether the required public access block settings are configured from account level. The rule is NON_COMPLIANT when the public access block settings are not configured from account level.</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1955,11 +2780,36 @@
           <t>Checks that the access granted by the Amazon S3 bucket is restricted to any of the AWS principals, federated users, service principals, IP addresses, or VPCs that you provide. The rule is COMPLIANT if a bucket policy is not present.</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1997,11 +2847,36 @@
           <t>Checks that your Amazon S3 buckets do not allow public write access. The rule checks the Block Public Access settings, the bucket policy, and the bucket access control list (ACL).</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr"/>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2039,11 +2914,36 @@
           <t>Checks whether direct internet access is disabled for an Amazon SageMaker notebook instance. The rule is NON_COMPLIANT if Amazon SageMaker notebook instances are internet-enabled.</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2081,11 +2981,36 @@
           <t>Checks whether the root user access key is available. The rule is compliant if the user access key does not exist.</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2123,11 +3048,36 @@
           <t>Checks whether GuardDuty is enabled. You can optionally verify that the results are centralized in a specific AWS Account.</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2165,11 +3115,36 @@
           <t>Checks that AWS Security Hub is enabled for an AWS Account. The rule is NON_COMPLIANT if AWS Security Hub is not enabled.</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2207,11 +3182,36 @@
           <t>Checks whether ACM Certificates in your account are marked for expiration within the specified number of days. Certificates provided by ACM are automatically renewed. ACM does not automatically renew certificates that you import.</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2249,11 +3249,36 @@
           <t>Checks if rule evaluates AWS Application Load Balancers (ALB) to ensure they are configured to drop http headers. The rule is NON_COMPLIANT if the value of routing.http.drop_invalid_header_fields.enabled is set to false.</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2291,11 +3316,36 @@
           <t>Checks whether HTTP to HTTPS redirection is configured on all HTTP listeners of Application Load Balancers. The rule is NON_COMPLIANT if one or more HTTP listeners of Application Load Balancer do not have HTTP to HTTPS redirection configured.</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2333,11 +3383,36 @@
           <t>This rule checks whether the Elastic Load Balancer(s) uses SSL certificates provided by AWS Certificate Manager. You must use an SSL or HTTPS listener with your Elastic Load Balancer to use this rule.</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2375,11 +3450,36 @@
           <t>Checks whether your Classic Load Balancer's listeners are configured with SSL or HTTPS</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2417,11 +3517,36 @@
           <t>Checks whether Amazon Redshift clusters require TLS/SSL encryption to connect to SQL clients. The rule is NON_COMPLIANT if any Amazon Redshift cluster has parameter require_SSL not set to true.</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2459,11 +3584,36 @@
           <t>Checks whether S3 buckets have policies that require requests to use Secure Socket Layer (SSL).</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
-      <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2501,11 +3651,36 @@
           <t>Checks that Internet gateways (IGWs) are only attached to an authorized Amazon Virtual Private Cloud (VPCs). The rule is NON_COMPLIANT if IGWs are not attached to an authorized VPC.</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr"/>
-      <c r="J48" t="inlineStr"/>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2543,11 +3718,36 @@
           <t>Checks whether AWS CloudTrail is configured to use the server side encryption (SSE) AWS Key Management Service (AWS KMS) customer master key (CMK) encryption. The rule is compliant if the KmsKeyId is defined.</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr"/>
-      <c r="K49" t="inlineStr"/>
-      <c r="L49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2585,11 +3785,36 @@
           <t>Checks whether a log group in Amazon CloudWatch Logs is encrypted. The rule is NON_COMPLIANT if CloudWatch Logs has log group without encryption enabled.</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2627,11 +3852,36 @@
           <t>Checks whether the Amazon EC2 instances in your account are managed by AWS Systems Manager.</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
-      <c r="J51" t="inlineStr"/>
-      <c r="K51" t="inlineStr"/>
-      <c r="L51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2669,11 +3919,36 @@
           <t>Checks whether the compliance status of the AWS Systems Manager association compliance is COMPLIANT or NON_COMPLIANT after the association execution on the instance. The rule is compliant if the field status is COMPLIANT.</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr"/>
-      <c r="L52" t="inlineStr"/>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2711,11 +3986,36 @@
           <t>Checks whether the Amazon EC2 instances in your account are managed by AWS Systems Manager.</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr"/>
-      <c r="L53" t="inlineStr"/>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2753,11 +4053,36 @@
           <t>Checks whether the compliance status of the AWS Systems Manager association compliance is COMPLIANT or NON_COMPLIANT after the association execution on the instance. The rule is compliant if the field status is COMPLIANT.</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr"/>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2795,11 +4120,36 @@
           <t>Checks whether the compliance status of the AWS Systems Manager patch compliance is COMPLIANT or NON_COMPLIANT after the patch installation on the instance. The rule is compliant if the field status is COMPLIANT.</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
-      <c r="J55" t="inlineStr"/>
-      <c r="K55" t="inlineStr"/>
-      <c r="L55" t="inlineStr"/>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2837,11 +4187,36 @@
           <t>Checks whether the account password policy for IAM users meets the specified requirements indicated in the parameters. This rule is NON_COMPLIANT if the account password policy does not meet the specified requirements.</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
-      <c r="K56" t="inlineStr"/>
-      <c r="L56" t="inlineStr"/>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr"/>
@@ -2851,11 +4226,36 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1"/>

</xml_diff>